<commit_message>
updated qPCR_setup to match worklist worktable labware
</commit_message>
<xml_diff>
--- a/tests/data/qPCR_setup/qPCR_Zach_plate1.xlsx
+++ b/tests/data/qPCR_setup/qPCR_Zach_plate1.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" iterateCount="1" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateCount="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="51">
   <si>
     <t>Row</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>1,28E-07</t>
-  </si>
-  <si>
-    <t>Tube</t>
   </si>
   <si>
     <t>K</t>
@@ -171,12 +168,6 @@
     <t>Sample location</t>
   </si>
   <si>
-    <t>96-well</t>
-  </si>
-  <si>
-    <t>384-well</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -184,6 +175,12 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>Tubes[003]</t>
+  </si>
+  <si>
+    <t>96 Well[004]</t>
   </si>
 </sst>
 </file>
@@ -501,7 +498,7 @@
   <dimension ref="A1:P127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="K43" sqref="K41:K127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,22 +535,22 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
         <v>41</v>
       </c>
-      <c r="L1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>42</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>43</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>44</v>
-      </c>
-      <c r="P1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -654,7 +651,7 @@
         <v>13</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L5">
         <v>12</v>
@@ -692,7 +689,7 @@
         <v>13</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L6">
         <v>12</v>
@@ -730,7 +727,7 @@
         <v>13</v>
       </c>
       <c r="K7" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L7">
         <v>12</v>
@@ -750,7 +747,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -762,13 +759,13 @@
         <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
         <v>13</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L8">
         <v>11</v>
@@ -788,7 +785,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -800,13 +797,13 @@
         <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
         <v>13</v>
       </c>
       <c r="K9" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L9">
         <v>11</v>
@@ -826,7 +823,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -838,13 +835,13 @@
         <v>11</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J10" t="s">
         <v>13</v>
       </c>
       <c r="K10" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L10">
         <v>11</v>
@@ -864,7 +861,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -876,13 +873,13 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J11" t="s">
         <v>13</v>
       </c>
       <c r="K11" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L11">
         <v>10</v>
@@ -902,7 +899,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -914,13 +911,13 @@
         <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J12" t="s">
         <v>13</v>
       </c>
       <c r="K12" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L12">
         <v>10</v>
@@ -940,7 +937,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -952,13 +949,13 @@
         <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J13" t="s">
         <v>13</v>
       </c>
       <c r="K13" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L13">
         <v>10</v>
@@ -978,7 +975,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -990,13 +987,13 @@
         <v>9</v>
       </c>
       <c r="I14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J14" t="s">
         <v>13</v>
       </c>
       <c r="K14" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L14">
         <v>9</v>
@@ -1016,7 +1013,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1028,13 +1025,13 @@
         <v>9</v>
       </c>
       <c r="I15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J15" t="s">
         <v>13</v>
       </c>
       <c r="K15" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L15">
         <v>9</v>
@@ -1054,7 +1051,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1066,13 +1063,13 @@
         <v>9</v>
       </c>
       <c r="I16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J16" t="s">
         <v>13</v>
       </c>
       <c r="K16" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L16">
         <v>9</v>
@@ -1092,7 +1089,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -1104,13 +1101,13 @@
         <v>8</v>
       </c>
       <c r="I17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J17" t="s">
         <v>13</v>
       </c>
       <c r="K17" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L17">
         <v>8</v>
@@ -1130,7 +1127,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1142,13 +1139,13 @@
         <v>8</v>
       </c>
       <c r="I18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J18" t="s">
         <v>13</v>
       </c>
       <c r="K18" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L18">
         <v>8</v>
@@ -1168,7 +1165,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1180,13 +1177,13 @@
         <v>8</v>
       </c>
       <c r="I19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J19" t="s">
         <v>13</v>
       </c>
       <c r="K19" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L19">
         <v>8</v>
@@ -1206,7 +1203,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -1218,13 +1215,13 @@
         <v>7</v>
       </c>
       <c r="I20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J20" t="s">
         <v>13</v>
       </c>
       <c r="K20" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L20">
         <v>7</v>
@@ -1244,7 +1241,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -1256,13 +1253,13 @@
         <v>7</v>
       </c>
       <c r="I21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J21" t="s">
         <v>13</v>
       </c>
       <c r="K21" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L21">
         <v>7</v>
@@ -1282,7 +1279,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1294,13 +1291,13 @@
         <v>7</v>
       </c>
       <c r="I22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J22" t="s">
         <v>13</v>
       </c>
       <c r="K22" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L22">
         <v>7</v>
@@ -1320,7 +1317,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -1332,13 +1329,13 @@
         <v>6</v>
       </c>
       <c r="I23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J23" t="s">
         <v>13</v>
       </c>
       <c r="K23" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L23">
         <v>6</v>
@@ -1358,7 +1355,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1370,13 +1367,13 @@
         <v>6</v>
       </c>
       <c r="I24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J24" t="s">
         <v>13</v>
       </c>
       <c r="K24" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L24">
         <v>6</v>
@@ -1396,7 +1393,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1408,13 +1405,13 @@
         <v>6</v>
       </c>
       <c r="I25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J25" t="s">
         <v>13</v>
       </c>
       <c r="K25" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L25">
         <v>6</v>
@@ -1434,7 +1431,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -1446,13 +1443,13 @@
         <v>5</v>
       </c>
       <c r="I26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J26" t="s">
         <v>13</v>
       </c>
       <c r="K26" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L26">
         <v>5</v>
@@ -1472,7 +1469,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -1484,13 +1481,13 @@
         <v>5</v>
       </c>
       <c r="I27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J27" t="s">
         <v>13</v>
       </c>
       <c r="K27" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L27">
         <v>5</v>
@@ -1510,7 +1507,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1522,13 +1519,13 @@
         <v>5</v>
       </c>
       <c r="I28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J28" t="s">
         <v>13</v>
       </c>
       <c r="K28" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L28">
         <v>5</v>
@@ -1548,7 +1545,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -1560,13 +1557,13 @@
         <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J29" t="s">
         <v>13</v>
       </c>
       <c r="K29" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L29">
         <v>4</v>
@@ -1586,7 +1583,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -1598,13 +1595,13 @@
         <v>4</v>
       </c>
       <c r="I30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J30" t="s">
         <v>13</v>
       </c>
       <c r="K30" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L30">
         <v>4</v>
@@ -1624,7 +1621,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1636,13 +1633,13 @@
         <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J31" t="s">
         <v>13</v>
       </c>
       <c r="K31" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L31">
         <v>4</v>
@@ -1662,7 +1659,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -1674,13 +1671,13 @@
         <v>3</v>
       </c>
       <c r="I32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J32" t="s">
         <v>13</v>
       </c>
       <c r="K32" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L32">
         <v>3</v>
@@ -1700,7 +1697,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1712,13 +1709,13 @@
         <v>3</v>
       </c>
       <c r="I33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J33" t="s">
         <v>13</v>
       </c>
       <c r="K33" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L33">
         <v>3</v>
@@ -1738,7 +1735,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1750,13 +1747,13 @@
         <v>3</v>
       </c>
       <c r="I34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J34" t="s">
         <v>13</v>
       </c>
       <c r="K34" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L34">
         <v>3</v>
@@ -1776,7 +1773,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -1788,13 +1785,13 @@
         <v>2</v>
       </c>
       <c r="I35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J35" t="s">
         <v>13</v>
       </c>
       <c r="K35" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L35">
         <v>2</v>
@@ -1814,7 +1811,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -1826,13 +1823,13 @@
         <v>2</v>
       </c>
       <c r="I36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J36" t="s">
         <v>13</v>
       </c>
       <c r="K36" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L36">
         <v>2</v>
@@ -1852,7 +1849,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1864,13 +1861,13 @@
         <v>2</v>
       </c>
       <c r="I37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J37" t="s">
         <v>13</v>
       </c>
       <c r="K37" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L37">
         <v>2</v>
@@ -1902,13 +1899,13 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J38" t="s">
         <v>13</v>
       </c>
       <c r="K38" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L38">
         <v>1</v>
@@ -1940,13 +1937,13 @@
         <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J39" t="s">
         <v>13</v>
       </c>
       <c r="K39" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L39">
         <v>1</v>
@@ -1978,13 +1975,13 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J40" t="s">
         <v>13</v>
       </c>
       <c r="K40" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L40">
         <v>1</v>
@@ -2010,7 +2007,7 @@
         <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I41" t="s">
         <v>12</v>
@@ -2019,7 +2016,7 @@
         <v>13</v>
       </c>
       <c r="K41" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L41">
         <v>1</v>
@@ -2045,7 +2042,7 @@
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I42" t="s">
         <v>12</v>
@@ -2054,7 +2051,7 @@
         <v>13</v>
       </c>
       <c r="K42" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L42">
         <v>1</v>
@@ -2080,7 +2077,7 @@
         <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I43" t="s">
         <v>12</v>
@@ -2089,7 +2086,7 @@
         <v>13</v>
       </c>
       <c r="K43" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L43">
         <v>1</v>
@@ -2115,7 +2112,7 @@
         <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I44" t="s">
         <v>12</v>
@@ -2124,7 +2121,7 @@
         <v>13</v>
       </c>
       <c r="K44" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L44">
         <v>2</v>
@@ -2150,7 +2147,7 @@
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I45" t="s">
         <v>12</v>
@@ -2159,7 +2156,7 @@
         <v>13</v>
       </c>
       <c r="K45" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L45">
         <v>2</v>
@@ -2185,7 +2182,7 @@
         <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I46" t="s">
         <v>12</v>
@@ -2194,7 +2191,7 @@
         <v>13</v>
       </c>
       <c r="K46" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L46">
         <v>2</v>
@@ -2214,13 +2211,13 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47">
         <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I47" t="s">
         <v>12</v>
@@ -2229,7 +2226,7 @@
         <v>13</v>
       </c>
       <c r="K47" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L47">
         <v>3</v>
@@ -2249,13 +2246,13 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B48">
         <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I48" t="s">
         <v>12</v>
@@ -2264,7 +2261,7 @@
         <v>13</v>
       </c>
       <c r="K48" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L48">
         <v>3</v>
@@ -2284,13 +2281,13 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49">
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I49" t="s">
         <v>12</v>
@@ -2299,7 +2296,7 @@
         <v>13</v>
       </c>
       <c r="K49" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L49">
         <v>3</v>
@@ -2319,13 +2316,13 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B50">
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I50" t="s">
         <v>12</v>
@@ -2334,7 +2331,7 @@
         <v>13</v>
       </c>
       <c r="K50" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L50">
         <v>4</v>
@@ -2354,13 +2351,13 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B51">
         <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I51" t="s">
         <v>12</v>
@@ -2369,7 +2366,7 @@
         <v>13</v>
       </c>
       <c r="K51" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L51">
         <v>4</v>
@@ -2389,13 +2386,13 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B52">
         <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I52" t="s">
         <v>12</v>
@@ -2404,7 +2401,7 @@
         <v>13</v>
       </c>
       <c r="K52" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L52">
         <v>4</v>
@@ -2424,13 +2421,13 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B53">
         <v>15</v>
       </c>
       <c r="C53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I53" t="s">
         <v>12</v>
@@ -2439,7 +2436,7 @@
         <v>13</v>
       </c>
       <c r="K53" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L53">
         <v>5</v>
@@ -2459,13 +2456,13 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B54">
         <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I54" t="s">
         <v>12</v>
@@ -2474,7 +2471,7 @@
         <v>13</v>
       </c>
       <c r="K54" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L54">
         <v>5</v>
@@ -2494,13 +2491,13 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B55">
         <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I55" t="s">
         <v>12</v>
@@ -2509,7 +2506,7 @@
         <v>13</v>
       </c>
       <c r="K55" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L55">
         <v>5</v>
@@ -2529,13 +2526,13 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B56">
         <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D56">
         <v>10</v>
@@ -2547,7 +2544,7 @@
         <v>13</v>
       </c>
       <c r="K56" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L56">
         <v>6</v>
@@ -2567,13 +2564,13 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B57">
         <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D57">
         <v>10</v>
@@ -2585,7 +2582,7 @@
         <v>13</v>
       </c>
       <c r="K57" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L57">
         <v>6</v>
@@ -2605,13 +2602,13 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B58">
         <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D58">
         <v>10</v>
@@ -2623,7 +2620,7 @@
         <v>13</v>
       </c>
       <c r="K58" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L58">
         <v>6</v>
@@ -2643,13 +2640,13 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B59">
         <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I59" t="s">
         <v>12</v>
@@ -2658,7 +2655,7 @@
         <v>13</v>
       </c>
       <c r="K59" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L59">
         <v>7</v>
@@ -2678,13 +2675,13 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B60">
         <v>11</v>
       </c>
       <c r="C60" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I60" t="s">
         <v>12</v>
@@ -2693,7 +2690,7 @@
         <v>13</v>
       </c>
       <c r="K60" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L60">
         <v>7</v>
@@ -2713,13 +2710,13 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B61">
         <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I61" t="s">
         <v>12</v>
@@ -2728,7 +2725,7 @@
         <v>13</v>
       </c>
       <c r="K61" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L61">
         <v>7</v>
@@ -2748,13 +2745,13 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B62">
         <v>15</v>
       </c>
       <c r="C62" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I62" t="s">
         <v>12</v>
@@ -2763,7 +2760,7 @@
         <v>13</v>
       </c>
       <c r="K62" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L62">
         <v>8</v>
@@ -2783,13 +2780,13 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B63">
         <v>14</v>
       </c>
       <c r="C63" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I63" t="s">
         <v>12</v>
@@ -2798,7 +2795,7 @@
         <v>13</v>
       </c>
       <c r="K63" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L63">
         <v>8</v>
@@ -2818,13 +2815,13 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B64">
         <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I64" t="s">
         <v>12</v>
@@ -2833,7 +2830,7 @@
         <v>13</v>
       </c>
       <c r="K64" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L64">
         <v>8</v>
@@ -2853,13 +2850,13 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B65">
         <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D65">
         <v>9</v>
@@ -2871,7 +2868,7 @@
         <v>13</v>
       </c>
       <c r="K65" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L65">
         <v>9</v>
@@ -2891,13 +2888,13 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B66">
         <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D66">
         <v>9</v>
@@ -2909,7 +2906,7 @@
         <v>13</v>
       </c>
       <c r="K66" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L66">
         <v>9</v>
@@ -2929,13 +2926,13 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B67">
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D67">
         <v>9</v>
@@ -2947,7 +2944,7 @@
         <v>13</v>
       </c>
       <c r="K67" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L67">
         <v>9</v>
@@ -2967,13 +2964,13 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B68">
         <v>12</v>
       </c>
       <c r="C68" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I68" t="s">
         <v>12</v>
@@ -2982,7 +2979,7 @@
         <v>13</v>
       </c>
       <c r="K68" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L68">
         <v>10</v>
@@ -3002,13 +2999,13 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B69">
         <v>11</v>
       </c>
       <c r="C69" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I69" t="s">
         <v>12</v>
@@ -3017,7 +3014,7 @@
         <v>13</v>
       </c>
       <c r="K69" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L69">
         <v>10</v>
@@ -3037,13 +3034,13 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B70">
         <v>10</v>
       </c>
       <c r="C70" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I70" t="s">
         <v>12</v>
@@ -3052,7 +3049,7 @@
         <v>13</v>
       </c>
       <c r="K70" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L70">
         <v>10</v>
@@ -3072,13 +3069,13 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B71">
         <v>15</v>
       </c>
       <c r="C71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I71" t="s">
         <v>12</v>
@@ -3087,7 +3084,7 @@
         <v>13</v>
       </c>
       <c r="K71" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L71">
         <v>11</v>
@@ -3107,13 +3104,13 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B72">
         <v>14</v>
       </c>
       <c r="C72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I72" t="s">
         <v>12</v>
@@ -3122,7 +3119,7 @@
         <v>13</v>
       </c>
       <c r="K72" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L72">
         <v>11</v>
@@ -3142,13 +3139,13 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B73">
         <v>13</v>
       </c>
       <c r="C73" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I73" t="s">
         <v>12</v>
@@ -3157,7 +3154,7 @@
         <v>13</v>
       </c>
       <c r="K73" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L73">
         <v>11</v>
@@ -3177,13 +3174,13 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B74">
         <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D74">
         <v>8</v>
@@ -3195,7 +3192,7 @@
         <v>13</v>
       </c>
       <c r="K74" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L74">
         <v>12</v>
@@ -3215,13 +3212,13 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B75">
         <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D75">
         <v>8</v>
@@ -3233,7 +3230,7 @@
         <v>13</v>
       </c>
       <c r="K75" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L75">
         <v>12</v>
@@ -3253,13 +3250,13 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B76">
         <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D76">
         <v>8</v>
@@ -3271,7 +3268,7 @@
         <v>13</v>
       </c>
       <c r="K76" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L76">
         <v>12</v>
@@ -3291,13 +3288,13 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B77">
         <v>12</v>
       </c>
       <c r="C77" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I77" t="s">
         <v>12</v>
@@ -3306,7 +3303,7 @@
         <v>13</v>
       </c>
       <c r="K77" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L77">
         <v>13</v>
@@ -3326,13 +3323,13 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B78">
         <v>11</v>
       </c>
       <c r="C78" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I78" t="s">
         <v>12</v>
@@ -3341,7 +3338,7 @@
         <v>13</v>
       </c>
       <c r="K78" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L78">
         <v>13</v>
@@ -3361,13 +3358,13 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B79">
         <v>10</v>
       </c>
       <c r="C79" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I79" t="s">
         <v>12</v>
@@ -3376,7 +3373,7 @@
         <v>13</v>
       </c>
       <c r="K79" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L79">
         <v>13</v>
@@ -3396,13 +3393,13 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B80">
         <v>15</v>
       </c>
       <c r="C80" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I80" t="s">
         <v>12</v>
@@ -3411,7 +3408,7 @@
         <v>13</v>
       </c>
       <c r="K80" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L80">
         <v>14</v>
@@ -3431,13 +3428,13 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B81">
         <v>14</v>
       </c>
       <c r="C81" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I81" t="s">
         <v>12</v>
@@ -3446,7 +3443,7 @@
         <v>13</v>
       </c>
       <c r="K81" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L81">
         <v>14</v>
@@ -3466,13 +3463,13 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B82">
         <v>13</v>
       </c>
       <c r="C82" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I82" t="s">
         <v>12</v>
@@ -3481,7 +3478,7 @@
         <v>13</v>
       </c>
       <c r="K82" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L82">
         <v>14</v>
@@ -3501,13 +3498,13 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B83">
         <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D83">
         <v>7</v>
@@ -3519,7 +3516,7 @@
         <v>13</v>
       </c>
       <c r="K83" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L83">
         <v>15</v>
@@ -3539,13 +3536,13 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B84">
         <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D84">
         <v>7</v>
@@ -3557,7 +3554,7 @@
         <v>13</v>
       </c>
       <c r="K84" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L84">
         <v>15</v>
@@ -3577,13 +3574,13 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B85">
         <v>4</v>
       </c>
       <c r="C85" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D85">
         <v>7</v>
@@ -3595,7 +3592,7 @@
         <v>13</v>
       </c>
       <c r="K85" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L85">
         <v>15</v>
@@ -3615,13 +3612,13 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B86">
         <v>12</v>
       </c>
       <c r="C86" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I86" t="s">
         <v>12</v>
@@ -3630,7 +3627,7 @@
         <v>13</v>
       </c>
       <c r="K86" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L86">
         <v>16</v>
@@ -3650,13 +3647,13 @@
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B87">
         <v>11</v>
       </c>
       <c r="C87" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I87" t="s">
         <v>12</v>
@@ -3665,7 +3662,7 @@
         <v>13</v>
       </c>
       <c r="K87" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L87">
         <v>16</v>
@@ -3685,13 +3682,13 @@
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B88">
         <v>10</v>
       </c>
       <c r="C88" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I88" t="s">
         <v>12</v>
@@ -3700,7 +3697,7 @@
         <v>13</v>
       </c>
       <c r="K88" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L88">
         <v>16</v>
@@ -3720,13 +3717,13 @@
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B89">
         <v>15</v>
       </c>
       <c r="C89" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I89" t="s">
         <v>12</v>
@@ -3735,7 +3732,7 @@
         <v>13</v>
       </c>
       <c r="K89" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L89">
         <v>17</v>
@@ -3755,13 +3752,13 @@
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B90">
         <v>14</v>
       </c>
       <c r="C90" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I90" t="s">
         <v>12</v>
@@ -3770,7 +3767,7 @@
         <v>13</v>
       </c>
       <c r="K90" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L90">
         <v>17</v>
@@ -3790,13 +3787,13 @@
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B91">
         <v>13</v>
       </c>
       <c r="C91" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I91" t="s">
         <v>12</v>
@@ -3805,7 +3802,7 @@
         <v>13</v>
       </c>
       <c r="K91" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L91">
         <v>17</v>
@@ -3825,13 +3822,13 @@
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B92">
         <v>6</v>
       </c>
       <c r="C92" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D92">
         <v>6</v>
@@ -3843,7 +3840,7 @@
         <v>13</v>
       </c>
       <c r="K92" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L92">
         <v>18</v>
@@ -3863,13 +3860,13 @@
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B93">
         <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D93">
         <v>6</v>
@@ -3881,7 +3878,7 @@
         <v>13</v>
       </c>
       <c r="K93" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L93">
         <v>18</v>
@@ -3901,13 +3898,13 @@
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B94">
         <v>4</v>
       </c>
       <c r="C94" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D94">
         <v>6</v>
@@ -3919,7 +3916,7 @@
         <v>13</v>
       </c>
       <c r="K94" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L94">
         <v>18</v>
@@ -3939,13 +3936,13 @@
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B95">
         <v>12</v>
       </c>
       <c r="C95" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I95" t="s">
         <v>12</v>
@@ -3954,7 +3951,7 @@
         <v>13</v>
       </c>
       <c r="K95" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L95">
         <v>19</v>
@@ -3974,13 +3971,13 @@
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B96">
         <v>11</v>
       </c>
       <c r="C96" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I96" t="s">
         <v>12</v>
@@ -3989,7 +3986,7 @@
         <v>13</v>
       </c>
       <c r="K96" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L96">
         <v>19</v>
@@ -4009,13 +4006,13 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B97">
         <v>10</v>
       </c>
       <c r="C97" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I97" t="s">
         <v>12</v>
@@ -4024,7 +4021,7 @@
         <v>13</v>
       </c>
       <c r="K97" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L97">
         <v>19</v>
@@ -4044,13 +4041,13 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B98">
         <v>15</v>
       </c>
       <c r="C98" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I98" t="s">
         <v>12</v>
@@ -4059,7 +4056,7 @@
         <v>13</v>
       </c>
       <c r="K98" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L98">
         <v>20</v>
@@ -4079,13 +4076,13 @@
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B99">
         <v>14</v>
       </c>
       <c r="C99" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I99" t="s">
         <v>12</v>
@@ -4094,7 +4091,7 @@
         <v>13</v>
       </c>
       <c r="K99" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L99">
         <v>20</v>
@@ -4114,13 +4111,13 @@
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B100">
         <v>13</v>
       </c>
       <c r="C100" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I100" t="s">
         <v>12</v>
@@ -4129,7 +4126,7 @@
         <v>13</v>
       </c>
       <c r="K100" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L100">
         <v>20</v>
@@ -4149,13 +4146,13 @@
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B101">
         <v>6</v>
       </c>
       <c r="C101" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D101">
         <v>5</v>
@@ -4167,7 +4164,7 @@
         <v>13</v>
       </c>
       <c r="K101" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L101">
         <v>21</v>
@@ -4187,13 +4184,13 @@
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B102">
         <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D102">
         <v>5</v>
@@ -4205,7 +4202,7 @@
         <v>13</v>
       </c>
       <c r="K102" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L102">
         <v>21</v>
@@ -4225,13 +4222,13 @@
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B103">
         <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D103">
         <v>5</v>
@@ -4243,7 +4240,7 @@
         <v>13</v>
       </c>
       <c r="K103" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L103">
         <v>21</v>
@@ -4263,13 +4260,13 @@
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B104">
         <v>12</v>
       </c>
       <c r="C104" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I104" t="s">
         <v>12</v>
@@ -4278,7 +4275,7 @@
         <v>13</v>
       </c>
       <c r="K104" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L104">
         <v>22</v>
@@ -4298,13 +4295,13 @@
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B105">
         <v>11</v>
       </c>
       <c r="C105" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I105" t="s">
         <v>12</v>
@@ -4313,7 +4310,7 @@
         <v>13</v>
       </c>
       <c r="K105" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L105">
         <v>22</v>
@@ -4333,13 +4330,13 @@
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B106">
         <v>10</v>
       </c>
       <c r="C106" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I106" t="s">
         <v>12</v>
@@ -4348,7 +4345,7 @@
         <v>13</v>
       </c>
       <c r="K106" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L106">
         <v>22</v>
@@ -4368,13 +4365,13 @@
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B107">
         <v>15</v>
       </c>
       <c r="C107" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I107" t="s">
         <v>12</v>
@@ -4383,7 +4380,7 @@
         <v>13</v>
       </c>
       <c r="K107" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L107">
         <v>23</v>
@@ -4403,13 +4400,13 @@
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B108">
         <v>14</v>
       </c>
       <c r="C108" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I108" t="s">
         <v>12</v>
@@ -4418,7 +4415,7 @@
         <v>13</v>
       </c>
       <c r="K108" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L108">
         <v>23</v>
@@ -4438,13 +4435,13 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B109">
         <v>13</v>
       </c>
       <c r="C109" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I109" t="s">
         <v>12</v>
@@ -4453,7 +4450,7 @@
         <v>13</v>
       </c>
       <c r="K109" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L109">
         <v>23</v>
@@ -4473,13 +4470,13 @@
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B110">
         <v>6</v>
       </c>
       <c r="C110" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D110">
         <v>4</v>
@@ -4491,7 +4488,7 @@
         <v>13</v>
       </c>
       <c r="K110" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L110">
         <v>24</v>
@@ -4511,13 +4508,13 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B111">
         <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D111">
         <v>4</v>
@@ -4529,7 +4526,7 @@
         <v>13</v>
       </c>
       <c r="K111" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L111">
         <v>24</v>
@@ -4549,13 +4546,13 @@
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B112">
         <v>4</v>
       </c>
       <c r="C112" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D112">
         <v>4</v>
@@ -4567,7 +4564,7 @@
         <v>13</v>
       </c>
       <c r="K112" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L112">
         <v>24</v>
@@ -4587,13 +4584,13 @@
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B113">
         <v>12</v>
       </c>
       <c r="C113" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I113" t="s">
         <v>12</v>
@@ -4602,7 +4599,7 @@
         <v>13</v>
       </c>
       <c r="K113" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L113">
         <v>25</v>
@@ -4622,13 +4619,13 @@
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B114">
         <v>11</v>
       </c>
       <c r="C114" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I114" t="s">
         <v>12</v>
@@ -4637,7 +4634,7 @@
         <v>13</v>
       </c>
       <c r="K114" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L114">
         <v>25</v>
@@ -4657,13 +4654,13 @@
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B115">
         <v>10</v>
       </c>
       <c r="C115" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I115" t="s">
         <v>12</v>
@@ -4672,7 +4669,7 @@
         <v>13</v>
       </c>
       <c r="K115" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L115">
         <v>25</v>
@@ -4692,13 +4689,13 @@
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B116">
         <v>15</v>
       </c>
       <c r="C116" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I116" t="s">
         <v>12</v>
@@ -4707,7 +4704,7 @@
         <v>13</v>
       </c>
       <c r="K116" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L116">
         <v>26</v>
@@ -4727,13 +4724,13 @@
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B117">
         <v>14</v>
       </c>
       <c r="C117" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I117" t="s">
         <v>12</v>
@@ -4742,7 +4739,7 @@
         <v>13</v>
       </c>
       <c r="K117" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L117">
         <v>26</v>
@@ -4762,13 +4759,13 @@
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B118">
         <v>13</v>
       </c>
       <c r="C118" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I118" t="s">
         <v>12</v>
@@ -4777,7 +4774,7 @@
         <v>13</v>
       </c>
       <c r="K118" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L118">
         <v>26</v>
@@ -4797,13 +4794,13 @@
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B119">
         <v>6</v>
       </c>
       <c r="C119" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D119">
         <v>3</v>
@@ -4815,7 +4812,7 @@
         <v>13</v>
       </c>
       <c r="K119" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L119">
         <v>27</v>
@@ -4835,13 +4832,13 @@
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B120">
         <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D120">
         <v>3</v>
@@ -4853,7 +4850,7 @@
         <v>13</v>
       </c>
       <c r="K120" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L120">
         <v>27</v>
@@ -4873,13 +4870,13 @@
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B121">
         <v>4</v>
       </c>
       <c r="C121" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D121">
         <v>3</v>
@@ -4891,7 +4888,7 @@
         <v>13</v>
       </c>
       <c r="K121" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L121">
         <v>27</v>
@@ -4911,13 +4908,13 @@
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B122">
         <v>12</v>
       </c>
       <c r="C122" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I122" t="s">
         <v>12</v>
@@ -4926,7 +4923,7 @@
         <v>13</v>
       </c>
       <c r="K122" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L122">
         <v>28</v>
@@ -4946,13 +4943,13 @@
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B123">
         <v>11</v>
       </c>
       <c r="C123" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I123" t="s">
         <v>12</v>
@@ -4961,7 +4958,7 @@
         <v>13</v>
       </c>
       <c r="K123" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L123">
         <v>28</v>
@@ -4981,13 +4978,13 @@
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B124">
         <v>10</v>
       </c>
       <c r="C124" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I124" t="s">
         <v>12</v>
@@ -4996,7 +4993,7 @@
         <v>13</v>
       </c>
       <c r="K124" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L124">
         <v>28</v>
@@ -5016,13 +5013,13 @@
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B125">
         <v>15</v>
       </c>
       <c r="C125" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I125" t="s">
         <v>12</v>
@@ -5031,7 +5028,7 @@
         <v>13</v>
       </c>
       <c r="K125" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L125">
         <v>29</v>
@@ -5051,13 +5048,13 @@
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B126">
         <v>14</v>
       </c>
       <c r="C126" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I126" t="s">
         <v>12</v>
@@ -5066,7 +5063,7 @@
         <v>13</v>
       </c>
       <c r="K126" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L126">
         <v>29</v>
@@ -5086,13 +5083,13 @@
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B127">
         <v>13</v>
       </c>
       <c r="C127" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I127" t="s">
         <v>12</v>
@@ -5101,7 +5098,7 @@
         <v>13</v>
       </c>
       <c r="K127" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L127">
         <v>29</v>
@@ -5247,7 +5244,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5311,7 +5308,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -5375,7 +5372,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -5439,7 +5436,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -5503,7 +5500,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -5567,7 +5564,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -5631,7 +5628,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -5695,7 +5692,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -5759,7 +5756,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -5823,7 +5820,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -6015,7 +6012,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -6079,7 +6076,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -6143,7 +6140,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B17">
         <v>16</v>

</xml_diff>